<commit_message>
changelog and credits update
</commit_message>
<xml_diff>
--- a/Credits.xlsx
+++ b/Credits.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="225">
   <si>
     <t>Credit Name Table</t>
   </si>
@@ -501,9 +501,6 @@
     <t>Xiafan Guanjun</t>
   </si>
   <si>
-    <t>Longship</t>
-  </si>
-  <si>
     <t>Andelsbevægelse</t>
   </si>
   <si>
@@ -534,9 +531,6 @@
     <t>Teutonic Order</t>
   </si>
   <si>
-    <t>Slaganz</t>
-  </si>
-  <si>
     <t>Agora</t>
   </si>
   <si>
@@ -657,9 +651,6 @@
     <t>Tarkhan</t>
   </si>
   <si>
-    <t>Intihuatana</t>
-  </si>
-  <si>
     <t>Chasqui</t>
   </si>
   <si>
@@ -703,13 +694,28 @@
   </si>
   <si>
     <t>Great Galleass(Firaxis)  / Fusta</t>
+  </si>
+  <si>
+    <t>Ulfhedinn</t>
+  </si>
+  <si>
+    <t>Danrell/Leugi</t>
+  </si>
+  <si>
+    <t>Asterix Rage</t>
+  </si>
+  <si>
+    <t>Langskib</t>
+  </si>
+  <si>
+    <t>Qullqa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -947,27 +953,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -977,17 +964,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1061,6 +1074,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1095,6 +1109,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1270,14 +1285,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
@@ -1295,36 +1310,36 @@
     <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="51"/>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="51"/>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="71" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="73"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="58"/>
       <c r="R1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1337,10 +1352,10 @@
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="56"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="43" t="s">
         <v>136</v>
       </c>
@@ -1376,7 +1391,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1401,8 +1416,10 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="2"/>
+      <c r="M3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N3" s="54"/>
       <c r="O3" s="2"/>
       <c r="P3" s="3"/>
       <c r="R3" s="9"/>
@@ -1410,7 +1427,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1419,8 +1436,8 @@
         <v>139</v>
       </c>
       <c r="D4" s="19"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="67"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="66"/>
       <c r="G4" s="50" t="s">
         <v>140</v>
       </c>
@@ -1435,8 +1452,10 @@
       <c r="L4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="2"/>
+      <c r="M4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N4" s="54"/>
       <c r="O4" s="2"/>
       <c r="P4" s="3"/>
       <c r="R4" s="26"/>
@@ -1444,7 +1463,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1455,10 +1474,10 @@
       <c r="D5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="61"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="50" t="s">
         <v>142</v>
       </c>
@@ -1469,8 +1488,10 @@
         <v>50</v>
       </c>
       <c r="L5" s="42"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="2"/>
+      <c r="M5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N5" s="54"/>
       <c r="O5" s="2"/>
       <c r="P5" s="3"/>
       <c r="R5" s="29"/>
@@ -1478,7 +1499,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1489,8 +1510,8 @@
         <v>143</v>
       </c>
       <c r="D6" s="19"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="50" t="s">
         <v>144</v>
       </c>
@@ -1507,8 +1528,10 @@
       <c r="L6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="2"/>
+      <c r="M6" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N6" s="54"/>
       <c r="O6" s="2"/>
       <c r="P6" s="3"/>
       <c r="R6" s="8" t="s">
@@ -1518,7 +1541,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1557,7 @@
       <c r="E7" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="50" t="s">
         <v>146</v>
       </c>
@@ -1552,9 +1575,9 @@
         <v>67</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N7" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="N7" s="54"/>
       <c r="O7" s="2"/>
       <c r="P7" s="3"/>
       <c r="R7" s="30" t="s">
@@ -1564,7 +1587,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1573,10 +1596,10 @@
         <v>147</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="61"/>
+      <c r="F8" s="62"/>
       <c r="G8" s="50" t="s">
         <v>148</v>
       </c>
@@ -1585,12 +1608,14 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="2"/>
+      <c r="M8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N8" s="54"/>
       <c r="O8" s="2"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1601,10 +1626,10 @@
       <c r="D9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="61"/>
+      <c r="E9" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="62"/>
       <c r="G9" s="50" t="s">
         <v>150</v>
       </c>
@@ -1621,8 +1646,10 @@
       <c r="L9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
+      <c r="M9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N9" s="54"/>
       <c r="O9" s="2"/>
       <c r="P9" s="3"/>
       <c r="R9" s="31"/>
@@ -1630,7 +1657,7 @@
       <c r="T9" s="31"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1639,8 +1666,8 @@
         <v>151</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="50" t="s">
         <v>152</v>
       </c>
@@ -1657,10 +1684,12 @@
         <v>50</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N10" s="54"/>
       <c r="O10" s="2"/>
       <c r="P10" s="3"/>
       <c r="R10" s="31"/>
@@ -1668,7 +1697,7 @@
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1677,8 +1706,8 @@
         <v>153</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="59"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
       <c r="G11" s="50" t="s">
         <v>154</v>
       </c>
@@ -1695,8 +1724,10 @@
       <c r="L11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="2"/>
+      <c r="M11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N11" s="54"/>
       <c r="O11" s="2"/>
       <c r="P11" s="3"/>
       <c r="R11" s="31"/>
@@ -1704,21 +1735,21 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="55" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="59"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="50" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>57</v>
@@ -1733,8 +1764,10 @@
       <c r="L12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="2"/>
+      <c r="M12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N12" s="54"/>
       <c r="O12" s="2"/>
       <c r="P12" s="3"/>
       <c r="R12" s="31"/>
@@ -1742,21 +1775,21 @@
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="68"/>
+      <c r="F13" s="70"/>
       <c r="G13" s="50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>57</v>
@@ -1771,8 +1804,10 @@
       <c r="L13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="2"/>
+      <c r="M13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N13" s="54"/>
       <c r="O13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1782,7 +1817,7 @@
       <c r="T13" s="31"/>
       <c r="U13" s="31"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1790,25 +1825,27 @@
         <v>127</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="61"/>
+      <c r="E14" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="62"/>
       <c r="G14" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="32"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="2"/>
+      <c r="M14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N14" s="54"/>
       <c r="O14" s="2"/>
       <c r="P14" s="3"/>
       <c r="R14" s="31"/>
@@ -1816,23 +1853,23 @@
       <c r="T14" s="31"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="61"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>76</v>
@@ -1845,28 +1882,30 @@
       <c r="L15" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="2"/>
+      <c r="M15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N15" s="54"/>
       <c r="O15" s="2"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="61"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>57</v>
@@ -1880,23 +1919,23 @@
         <v>67</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="54"/>
       <c r="O16" s="2"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D17" s="19"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="50" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>57</v>
@@ -1911,50 +1950,54 @@
       <c r="L17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="2"/>
+      <c r="M17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N17" s="54"/>
       <c r="O17" s="2"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="50" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="65"/>
+      <c r="F18" s="73"/>
       <c r="G18" s="49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="32"/>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="2"/>
+      <c r="M18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N18" s="54"/>
       <c r="O18" s="2"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="50" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D19" s="20"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="66"/>
       <c r="G19" s="50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="32"/>
@@ -1967,28 +2010,30 @@
       <c r="L19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M19" s="1"/>
-      <c r="N19" s="2"/>
+      <c r="M19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N19" s="54"/>
       <c r="O19" s="2"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="50" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="61"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="50" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>51</v>
@@ -2003,26 +2048,28 @@
       <c r="L20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="2"/>
+      <c r="M20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N20" s="54"/>
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" s="19"/>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="61"/>
+      <c r="F21" s="62"/>
       <c r="G21" s="50" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>57</v>
@@ -2037,54 +2084,58 @@
       <c r="L21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="2"/>
+      <c r="M21" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N21" s="54"/>
       <c r="O21" s="2"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="62" t="s">
+      <c r="E22" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="61"/>
+      <c r="F22" s="62"/>
       <c r="G22" s="50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="32"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="2"/>
+      <c r="M22" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N22" s="54"/>
       <c r="O22" s="2"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D23" s="19"/>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="68"/>
+      <c r="F23" s="70"/>
       <c r="G23" s="50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>88</v>
@@ -2097,28 +2148,30 @@
       <c r="L23" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="2"/>
+      <c r="M23" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N23" s="54"/>
       <c r="O23" s="2"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="50" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="62" t="s">
+      <c r="E24" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="61"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="50" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>88</v>
@@ -2133,28 +2186,30 @@
       <c r="L24" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="2"/>
+      <c r="M24" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N24" s="54"/>
       <c r="O24" s="2"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="F25" s="61"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="50" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>92</v>
@@ -2169,30 +2224,30 @@
       <c r="L25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M25" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N25" s="2"/>
+      <c r="M25" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N25" s="54"/>
       <c r="O25" s="2"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="61"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="50" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>65</v>
@@ -2205,32 +2260,30 @@
       <c r="L26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M26" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="M26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N26" s="54"/>
       <c r="O26" s="2"/>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="61"/>
+      <c r="F27" s="62"/>
       <c r="G27" s="50" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>93</v>
@@ -2243,26 +2296,26 @@
       <c r="L27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M27" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N27" s="2"/>
+      <c r="M27" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N27" s="54"/>
       <c r="O27" s="2"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D28" s="19"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="59"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68"/>
       <c r="G28" s="50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="32"/>
@@ -2271,40 +2324,44 @@
       </c>
       <c r="K28" s="32"/>
       <c r="L28" s="34"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="2"/>
+      <c r="M28" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N28" s="54"/>
       <c r="O28" s="2"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="50" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="61"/>
+      <c r="F29" s="62"/>
       <c r="G29" s="50" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="32"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="2"/>
+      <c r="M29" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N29" s="54"/>
       <c r="O29" s="21"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -2312,17 +2369,17 @@
         <v>127</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="62" t="s">
+      <c r="E30" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="61"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>57</v>
@@ -2335,26 +2392,26 @@
       <c r="L30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="M30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N30" s="54"/>
       <c r="O30" s="2"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="50" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D31" s="19"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="59"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
       <c r="G31" s="50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="32"/>
@@ -2364,29 +2421,29 @@
         <v>100</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N31" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="N31" s="54"/>
       <c r="O31" s="2"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="50" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="61"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="50" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>63</v>
@@ -2401,28 +2458,30 @@
       <c r="L32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="M32" s="1"/>
-      <c r="N32" s="2"/>
+      <c r="M32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N32" s="54"/>
       <c r="O32" s="2"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="62" t="s">
+      <c r="E33" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="61"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H33" t="s">
         <v>104</v>
@@ -2433,12 +2492,14 @@
       </c>
       <c r="K33" s="35"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="2"/>
+      <c r="M33" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N33" s="54"/>
       <c r="O33" s="2"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2446,17 +2507,17 @@
         <v>127</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="61"/>
+      <c r="E34" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="62"/>
       <c r="G34" s="50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="32"/>
@@ -2464,17 +2525,17 @@
       <c r="K34" s="13"/>
       <c r="L34" s="10"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="2"/>
+      <c r="N34" s="54"/>
       <c r="O34" s="2"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D35" s="52"/>
       <c r="E35" s="63" t="s">
@@ -2482,7 +2543,7 @@
       </c>
       <c r="F35" s="64"/>
       <c r="G35" s="49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>59</v>
@@ -2497,28 +2558,30 @@
       <c r="L35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="2"/>
+      <c r="M35" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N35" s="54"/>
       <c r="O35" s="2"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="61"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>59</v>
@@ -2532,31 +2595,29 @@
         <v>78</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="N36" s="54"/>
       <c r="O36" s="2"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="62" t="s">
+      <c r="E37" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="61"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>57</v>
@@ -2571,24 +2632,26 @@
       <c r="L37" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="M37" s="1"/>
-      <c r="N37" s="2"/>
+      <c r="M37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N37" s="54"/>
       <c r="O37" s="2"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="50" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D38" s="19"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="59"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="68"/>
       <c r="G38" s="50" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>80</v>
@@ -2603,24 +2666,28 @@
       <c r="L38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
+      <c r="M38" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N38" s="54"/>
+      <c r="O38" s="55" t="s">
+        <v>80</v>
+      </c>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="50" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D39" s="19"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="59"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="68"/>
       <c r="G39" s="50" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>59</v>
@@ -2633,28 +2700,30 @@
       <c r="L39" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="M39" s="1"/>
-      <c r="N39" s="2"/>
+      <c r="M39" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N39" s="54"/>
       <c r="O39" s="2"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="50" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="60" t="s">
+      <c r="E40" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="61"/>
+      <c r="F40" s="62"/>
       <c r="G40" s="50" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>51</v>
@@ -2670,29 +2739,29 @@
         <v>78</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N40" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="N40" s="54"/>
       <c r="O40" s="2"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="50" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="62" t="s">
+      <c r="E41" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="61"/>
+      <c r="F41" s="62"/>
       <c r="G41" s="50" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>89</v>
@@ -2707,28 +2776,30 @@
       <c r="L41" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="2"/>
+      <c r="M41" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N41" s="54"/>
       <c r="O41" s="2"/>
       <c r="P41" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="50" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D42" s="19"/>
-      <c r="E42" s="62" t="s">
+      <c r="E42" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="61"/>
+      <c r="F42" s="62"/>
       <c r="G42" s="50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>57</v>
@@ -2741,28 +2812,30 @@
       <c r="L42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M42" s="1"/>
-      <c r="N42" s="2"/>
+      <c r="M42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N42" s="54"/>
       <c r="O42" s="2"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="50" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E43" s="60" t="s">
+      <c r="E43" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="F43" s="61"/>
+      <c r="F43" s="62"/>
       <c r="G43" s="50" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>71</v>
@@ -2777,24 +2850,26 @@
       <c r="L43" t="s">
         <v>71</v>
       </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="2"/>
+      <c r="M43" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N43" s="54"/>
       <c r="O43" s="2"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D44" s="19"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="59"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68"/>
       <c r="G44" s="50" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>51</v>
@@ -2809,28 +2884,30 @@
       <c r="L44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="2"/>
+      <c r="M44" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N44" s="54"/>
       <c r="O44" s="2"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="43" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="56"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>57</v>
@@ -2846,25 +2923,25 @@
         <v>50</v>
       </c>
       <c r="M45" s="4"/>
-      <c r="N45" s="5"/>
+      <c r="N45" s="54"/>
       <c r="O45" s="5"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="47" spans="1:16">
-      <c r="A47" s="57" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="45"/>
       <c r="I47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
         <v>57</v>
       </c>
@@ -2879,7 +2956,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
         <v>50</v>
       </c>
@@ -2894,7 +2971,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>51</v>
       </c>
@@ -2909,7 +2986,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>62</v>
       </c>
@@ -2921,7 +2998,7 @@
       </c>
       <c r="G51" s="28"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>71</v>
       </c>
@@ -2932,7 +3009,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>99</v>
       </c>
@@ -2943,7 +3020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -2955,7 +3032,7 @@
       </c>
       <c r="G54" s="26"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2967,7 +3044,7 @@
       </c>
       <c r="G55" s="26"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -2978,7 +3055,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>67</v>
       </c>
@@ -2989,7 +3066,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -3001,7 +3078,7 @@
       </c>
       <c r="G58" s="28"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -3013,20 +3090,20 @@
       </c>
       <c r="G59" s="26"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
       <c r="D60" t="s">
         <v>85</v>
       </c>
-      <c r="F60" s="54" t="s">
+      <c r="F60" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="G60" s="54"/>
-      <c r="H60" s="54"/>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="G60" s="74"/>
+      <c r="H60" s="74"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3038,18 +3115,46 @@
       </c>
       <c r="G61" s="28"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3062,39 +3167,11 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
@@ -3102,24 +3179,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>